<commit_message>
adding new files to Advanced RestAssured Framework
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/BookingData.xlsx
+++ b/src/test/resources/test-data/BookingData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="17235" windowHeight="5460"/>
+    <workbookView xWindow="4320" yWindow="1905" windowWidth="15810" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>First Name</t>
   </si>
@@ -39,12 +40,6 @@
     <t>Additional Needs</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Waters</t>
-  </si>
-  <si>
     <t>2025-02-17</t>
   </si>
   <si>
@@ -76,6 +71,15 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>mbm</t>
+  </si>
+  <si>
+    <t>mannepalli</t>
   </si>
 </sst>
 </file>
@@ -423,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H12"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +444,7 @@
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,51 +466,60 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>